<commit_message>
se conecta todos los equipos de la lista y se extrae informacion correctamente
</commit_message>
<xml_diff>
--- a/Network_Devices_List.xlsx
+++ b/Network_Devices_List.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F2"/>
+  <dimension ref="A1:F3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -464,30 +464,62 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
+          <t>Mikrotik-Site-1</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>CHR</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>Desconocido</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>6.43.12 (stable)</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>192.168.240.133</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>Conectado</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
           <t>Mikrotik-Site-2</t>
         </is>
       </c>
-      <c r="B2" t="inlineStr">
+      <c r="B3" t="inlineStr">
         <is>
           <t>CHR</t>
         </is>
       </c>
-      <c r="C2" t="inlineStr">
+      <c r="C3" t="inlineStr">
         <is>
           <t>Desconocido</t>
         </is>
       </c>
-      <c r="D2" t="inlineStr">
+      <c r="D3" t="inlineStr">
         <is>
           <t>6.43.12 (stable)</t>
         </is>
       </c>
-      <c r="E2" t="inlineStr">
+      <c r="E3" t="inlineStr">
         <is>
           <t>192.168.240.134</t>
         </is>
       </c>
-      <c r="F2" t="inlineStr">
+      <c r="F3" t="inlineStr">
         <is>
           <t>Conectado</t>
         </is>

</xml_diff>